<commit_message>
working sript for multi substrat mm
</commit_message>
<xml_diff>
--- a/Fehlerfortpflanzunganalyse/Daten/Rohdaten/Plate_Reader/Kinetik-Messungen/r1/r1_NAD_PD_mod.xlsx
+++ b/Fehlerfortpflanzunganalyse/Daten/Rohdaten/Plate_Reader/Kinetik-Messungen/r1/r1_NAD_PD_mod.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="NAD (500 mM PD)" sheetId="1" r:id="rId1"/>
-    <sheet name="PD (5 mM NAD)" sheetId="2" r:id="rId2"/>
+    <sheet name="NAD_PD_500nM" sheetId="1" r:id="rId1"/>
+    <sheet name="PD_NAD_5nM" sheetId="2" r:id="rId2"/>
     <sheet name="Ergebnisse" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
@@ -3419,6 +3419,9 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="str">
+        <v/>
+      </c>
       <c r="B2" t="str">
         <v>Time [s]</v>
       </c>
@@ -5290,7 +5293,7 @@
         <v>0.374</v>
       </c>
       <c r="AZ13" t="str">
-        <v>0.378_x000d_</v>
+        <v>0.378</v>
       </c>
     </row>
     <row r="14">

</xml_diff>